<commit_message>
0.1.14: Enable METHOD spoilling function.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorKtTelegramProcessStructure.xlsx
+++ b/meta/program/BlancoRestGeneratorKtTelegramProcessStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuji/projects/blanco/blancoRestGeneratorKt/meta/program/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6941E5E-58D5-8349-9EAD-18499ED87F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E34F55A-488B-5A4A-9B78-8B180E547B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6880" yWindow="500" windowWidth="16700" windowHeight="17480" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -931,7 +931,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1081,67 +1081,70 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1535,7 +1538,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1579,7 +1582,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1604,10 +1607,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1780,23 +1783,23 @@
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="71"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="68"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="68"/>
-      <c r="B20" s="69"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="71"/>
+      <c r="A20" s="65"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="68"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
@@ -1833,29 +1836,29 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="68" t="s">
+      <c r="A25" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="74" t="s">
+      <c r="C25" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="74" t="s">
+      <c r="D25" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="74" t="s">
+      <c r="E25" s="71" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="28"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="68"/>
-      <c r="B26" s="68"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
+      <c r="A26" s="65"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="71"/>
       <c r="F26" s="29"/>
     </row>
     <row r="27" spans="1:6">
@@ -1893,7 +1896,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="32">
-        <f t="shared" ref="A29:A51" si="0">A28+1</f>
+        <f t="shared" ref="A29:A52" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="33" t="s">
@@ -1903,10 +1906,10 @@
         <v>23</v>
       </c>
       <c r="D29" s="34"/>
-      <c r="E29" s="72" t="s">
+      <c r="E29" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="73"/>
+      <c r="F29" s="70"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="32">
@@ -1920,10 +1923,10 @@
         <v>30</v>
       </c>
       <c r="D30" s="45"/>
-      <c r="E30" s="64" t="s">
+      <c r="E30" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="65"/>
+      <c r="F30" s="60"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="32">
@@ -1971,10 +1974,10 @@
         <v>30</v>
       </c>
       <c r="D33" s="34"/>
-      <c r="E33" s="66" t="s">
+      <c r="E33" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="67"/>
+      <c r="F33" s="62"/>
     </row>
     <row r="34" spans="1:7" ht="50" customHeight="1">
       <c r="A34" s="32">
@@ -1988,10 +1991,10 @@
         <v>30</v>
       </c>
       <c r="D34" s="34"/>
-      <c r="E34" s="66" t="s">
+      <c r="E34" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="F34" s="67"/>
+      <c r="F34" s="62"/>
     </row>
     <row r="35" spans="1:7" s="49" customFormat="1" ht="45">
       <c r="A35" s="32">
@@ -2007,10 +2010,10 @@
       <c r="D35" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="62" t="s">
+      <c r="E35" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="63"/>
+      <c r="F35" s="64"/>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" s="49" customFormat="1" ht="45">
@@ -2027,10 +2030,10 @@
       <c r="D36" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="62" t="s">
+      <c r="E36" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="F36" s="63"/>
+      <c r="F36" s="64"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" s="49" customFormat="1" ht="45">
@@ -2047,10 +2050,10 @@
       <c r="D37" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="E37" s="62" t="s">
+      <c r="E37" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="F37" s="63"/>
+      <c r="F37" s="64"/>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7">
@@ -2067,10 +2070,10 @@
       <c r="D38" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="64" t="s">
+      <c r="E38" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="F38" s="65"/>
+      <c r="F38" s="60"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="32">
@@ -2086,10 +2089,10 @@
       <c r="D39" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="E39" s="64" t="s">
+      <c r="E39" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="F39" s="65"/>
+      <c r="F39" s="60"/>
     </row>
     <row r="40" spans="1:7" s="49" customFormat="1" ht="15">
       <c r="A40" s="32">
@@ -2105,10 +2108,10 @@
       <c r="D40" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="E40" s="57" t="s">
+      <c r="E40" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="58"/>
+      <c r="F40" s="74"/>
       <c r="G40"/>
     </row>
     <row r="41" spans="1:7" s="49" customFormat="1" ht="15">
@@ -2123,10 +2126,10 @@
         <v>23</v>
       </c>
       <c r="D41" s="48"/>
-      <c r="E41" s="57" t="s">
+      <c r="E41" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="58"/>
+      <c r="F41" s="74"/>
       <c r="G41"/>
     </row>
     <row r="42" spans="1:7" s="49" customFormat="1" ht="45" customHeight="1">
@@ -2143,10 +2146,10 @@
       <c r="D42" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="57" t="s">
+      <c r="E42" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="F42" s="61"/>
+      <c r="F42" s="73"/>
       <c r="G42"/>
     </row>
     <row r="43" spans="1:7" s="49" customFormat="1" ht="45">
@@ -2163,10 +2166,10 @@
       <c r="D43" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="E43" s="57" t="s">
+      <c r="E43" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="F43" s="58"/>
+      <c r="F43" s="74"/>
       <c r="G43"/>
     </row>
     <row r="44" spans="1:7" s="49" customFormat="1" ht="45">
@@ -2183,10 +2186,10 @@
       <c r="D44" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="E44" s="59" t="s">
+      <c r="E44" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="F44" s="60"/>
+      <c r="F44" s="78"/>
       <c r="G44"/>
     </row>
     <row r="45" spans="1:7" s="49" customFormat="1" ht="90">
@@ -2194,7 +2197,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B45" s="75" t="s">
+      <c r="B45" s="57" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="56" t="s">
@@ -2203,10 +2206,10 @@
       <c r="D45" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="E45" s="76" t="s">
+      <c r="E45" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="F45" s="77"/>
+      <c r="F45" s="76"/>
       <c r="G45"/>
     </row>
     <row r="46" spans="1:7">
@@ -2274,10 +2277,10 @@
         <v>30</v>
       </c>
       <c r="D49" s="55"/>
-      <c r="E49" s="57" t="s">
+      <c r="E49" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="F49" s="58"/>
+      <c r="F49" s="74"/>
       <c r="G49"/>
     </row>
     <row r="50" spans="1:7" s="49" customFormat="1" ht="15">
@@ -2292,10 +2295,10 @@
         <v>30</v>
       </c>
       <c r="D50" s="55"/>
-      <c r="E50" s="57" t="s">
+      <c r="E50" s="72" t="s">
         <v>78</v>
       </c>
-      <c r="F50" s="58"/>
+      <c r="F50" s="74"/>
       <c r="G50"/>
     </row>
     <row r="51" spans="1:7" s="49" customFormat="1" ht="15">
@@ -2310,30 +2313,51 @@
         <v>30</v>
       </c>
       <c r="D51" s="55"/>
-      <c r="E51" s="57" t="s">
+      <c r="E51" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="F51" s="58"/>
+      <c r="F51" s="74"/>
       <c r="G51"/>
     </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="46"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="35"/>
+    <row r="52" spans="1:7" s="49" customFormat="1">
+      <c r="A52" s="32"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="63"/>
+      <c r="F52" s="64"/>
+      <c r="G52"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="24"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="37"/>
+      <c r="A53" s="46"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="35"/>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="24"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="29">
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="A25:A26"/>
@@ -2341,27 +2365,16 @@
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E45:F45"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">

</xml_diff>